<commit_message>
Added frequency as a decision variable to continuous model
</commit_message>
<xml_diff>
--- a/output/line_data.xlsx
+++ b/output/line_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vegardvk\vscodeProjects\bernstein\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501D868C-793C-41B1-87C3-B0842D612E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA9943B-BEF2-46B3-BBAA-E0CA4CB27BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{DC188162-EFF5-47E3-B49E-82E8905BA224}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="38040" xr2:uid="{DC188162-EFF5-47E3-B49E-82E8905BA224}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>10000</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Siste versjon brukt i EEM-artikkel
</commit_message>
<xml_diff>
--- a/output/line_data.xlsx
+++ b/output/line_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vegardvk\vscodeProjects\bernstein\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524E00EF-4393-42FC-9E13-F768E0CEDAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E170E52A-492F-493F-A204-43377083599A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC188162-EFF5-47E3-B49E-82E8905BA224}"/>
+    <workbookView xWindow="6405" yWindow="5040" windowWidth="11415" windowHeight="9000" xr2:uid="{DC188162-EFF5-47E3-B49E-82E8905BA224}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="old" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>area_from</t>
   </si>
@@ -424,11 +425,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C888AE7-C05B-4F81-BD98-733729A454AF}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42169524-6BD6-479D-A4BF-29A507AEEE16}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>